<commit_message>
found perfect triggers and refactored function
</commit_message>
<xml_diff>
--- a/app/Spreadsheets/internal/AddressMapVisualUnMapReference.xlsx
+++ b/app/Spreadsheets/internal/AddressMapVisualUnMapReference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgunter\Google Drive\Sphinx\Bone\Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgunter\PycharmProjects\MP2ASCII\app\Spreadsheets\internal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="288">
   <si>
     <t>SPORT</t>
   </si>
@@ -1714,8 +1714,8 @@
   <dimension ref="A1:N886"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A696" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H719" sqref="H719"/>
+      <pane ySplit="1" topLeftCell="A570" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A606" sqref="A606:XFD606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17355,41 +17355,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A489" s="1" t="s">
+    <row r="489" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A489" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B489" s="1" t="s">
+      <c r="B489" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C489" s="1">
+      <c r="C489" s="3">
         <v>17</v>
       </c>
-      <c r="D489" s="1">
-        <v>1</v>
-      </c>
-      <c r="E489" s="1">
-        <v>2</v>
-      </c>
-      <c r="F489" s="1">
-        <v>1</v>
-      </c>
-      <c r="G489" s="1">
-        <v>1</v>
-      </c>
-      <c r="H489" s="1">
-        <v>0</v>
-      </c>
-      <c r="I489" s="1">
-        <v>0</v>
-      </c>
-      <c r="J489" s="1" t="s">
+      <c r="D489" s="3">
+        <v>1</v>
+      </c>
+      <c r="E489" s="3">
+        <v>2</v>
+      </c>
+      <c r="F489" s="3">
+        <v>1</v>
+      </c>
+      <c r="G489" s="3">
+        <v>1</v>
+      </c>
+      <c r="H489" s="3">
+        <v>0</v>
+      </c>
+      <c r="I489" s="3">
+        <v>0</v>
+      </c>
+      <c r="J489" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K489" s="1" t="s">
+      <c r="K489" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L489" s="1">
+      <c r="L489" s="3">
         <v>0</v>
       </c>
     </row>
@@ -17431,73 +17431,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A491" t="s">
+    <row r="491" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A491" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B491" t="s">
+      <c r="B491" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C491">
+      <c r="C491" s="1">
         <v>19</v>
       </c>
-      <c r="D491">
-        <v>1</v>
-      </c>
-      <c r="E491">
-        <v>2</v>
-      </c>
-      <c r="F491">
-        <v>1</v>
-      </c>
-      <c r="G491">
-        <v>3</v>
-      </c>
-      <c r="H491">
-        <v>0</v>
-      </c>
-      <c r="I491">
-        <v>0</v>
-      </c>
-      <c r="K491" t="s">
+      <c r="D491" s="1">
+        <v>1</v>
+      </c>
+      <c r="E491" s="1">
+        <v>2</v>
+      </c>
+      <c r="F491" s="1">
+        <v>1</v>
+      </c>
+      <c r="G491" s="1">
+        <v>3</v>
+      </c>
+      <c r="H491" s="1">
+        <v>0</v>
+      </c>
+      <c r="I491" s="1">
+        <v>0</v>
+      </c>
+      <c r="K491" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L491">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="492" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
+      <c r="L491" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A492" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B492" t="s">
+      <c r="B492" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C492">
+      <c r="C492" s="1">
         <v>20</v>
       </c>
-      <c r="D492">
-        <v>1</v>
-      </c>
-      <c r="E492">
-        <v>2</v>
-      </c>
-      <c r="F492">
-        <v>1</v>
-      </c>
-      <c r="G492">
-        <v>4</v>
-      </c>
-      <c r="H492" t="s">
+      <c r="D492" s="1">
+        <v>1</v>
+      </c>
+      <c r="E492" s="1">
+        <v>2</v>
+      </c>
+      <c r="F492" s="1">
+        <v>1</v>
+      </c>
+      <c r="G492" s="1">
+        <v>4</v>
+      </c>
+      <c r="H492" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I492">
-        <v>0</v>
-      </c>
-      <c r="K492" t="s">
+      <c r="I492" s="1">
+        <v>0</v>
+      </c>
+      <c r="K492" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L492">
+      <c r="L492" s="1">
         <v>0</v>
       </c>
     </row>
@@ -18942,41 +18942,41 @@
         <v>64</v>
       </c>
     </row>
-    <row r="538" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A538" t="s">
+    <row r="538" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A538" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B538" t="s">
+      <c r="B538" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C538">
+      <c r="C538" s="1">
         <v>12</v>
       </c>
-      <c r="D538">
-        <v>1</v>
-      </c>
-      <c r="E538">
-        <v>1</v>
-      </c>
-      <c r="F538">
-        <v>3</v>
-      </c>
-      <c r="G538">
-        <v>4</v>
-      </c>
-      <c r="H538" t="s">
+      <c r="D538" s="1">
+        <v>1</v>
+      </c>
+      <c r="E538" s="1">
+        <v>1</v>
+      </c>
+      <c r="F538" s="1">
+        <v>3</v>
+      </c>
+      <c r="G538" s="1">
+        <v>4</v>
+      </c>
+      <c r="H538" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I538">
-        <v>0</v>
-      </c>
-      <c r="K538">
-        <v>0</v>
-      </c>
-      <c r="L538">
-        <v>0</v>
-      </c>
-      <c r="M538" t="s">
+      <c r="I538" s="1">
+        <v>0</v>
+      </c>
+      <c r="K538" s="1">
+        <v>0</v>
+      </c>
+      <c r="L538" s="1">
+        <v>0</v>
+      </c>
+      <c r="M538" s="1" t="s">
         <v>148</v>
       </c>
     </row>
@@ -20716,7 +20716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="593" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A593" t="s">
         <v>154</v>
       </c>
@@ -20751,7 +20751,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="595" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A595" s="1" t="s">
         <v>154</v>
       </c>
@@ -20789,7 +20789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="596" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A596" t="s">
         <v>154</v>
       </c>
@@ -20827,7 +20827,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="597" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A597" s="1" t="s">
         <v>154</v>
       </c>
@@ -20865,7 +20865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="598" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A598" s="1" t="s">
         <v>154</v>
       </c>
@@ -20900,45 +20900,48 @@
         <v>27</v>
       </c>
     </row>
-    <row r="599" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A599" t="s">
+    <row r="599" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A599" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B599" t="s">
+      <c r="B599" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C599">
+      <c r="C599" s="1">
         <v>12</v>
       </c>
-      <c r="D599">
-        <v>1</v>
-      </c>
-      <c r="E599">
-        <v>1</v>
-      </c>
-      <c r="F599">
-        <v>3</v>
-      </c>
-      <c r="G599">
-        <v>4</v>
-      </c>
-      <c r="H599" t="s">
+      <c r="D599" s="1">
+        <v>1</v>
+      </c>
+      <c r="E599" s="1">
+        <v>1</v>
+      </c>
+      <c r="F599" s="1">
+        <v>3</v>
+      </c>
+      <c r="G599" s="1">
+        <v>4</v>
+      </c>
+      <c r="H599" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I599">
-        <v>0</v>
-      </c>
-      <c r="K599">
-        <v>0</v>
-      </c>
-      <c r="L599">
-        <v>0</v>
-      </c>
-      <c r="M599" t="s">
+      <c r="I599" s="1">
+        <v>0</v>
+      </c>
+      <c r="K599" s="1">
+        <v>0</v>
+      </c>
+      <c r="L599" s="1">
+        <v>0</v>
+      </c>
+      <c r="M599" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="601" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N599" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="601" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A601" t="s">
         <v>154</v>
       </c>
@@ -20973,7 +20976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="602" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A602" t="s">
         <v>154</v>
       </c>
@@ -21008,7 +21011,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="603" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A603" t="s">
         <v>154</v>
       </c>
@@ -21043,7 +21046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="604" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A604" t="s">
         <v>154</v>
       </c>
@@ -21078,45 +21081,45 @@
         <v>27</v>
       </c>
     </row>
-    <row r="606" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A606" s="1" t="s">
+    <row r="606" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A606" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B606" s="1" t="s">
+      <c r="B606" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C606" s="1">
+      <c r="C606" s="3">
         <v>17</v>
       </c>
-      <c r="D606" s="1">
-        <v>1</v>
-      </c>
-      <c r="E606" s="1">
-        <v>2</v>
-      </c>
-      <c r="F606" s="1">
-        <v>1</v>
-      </c>
-      <c r="G606" s="1">
-        <v>1</v>
-      </c>
-      <c r="H606" s="1">
-        <v>0</v>
-      </c>
-      <c r="I606" s="1">
-        <v>0</v>
-      </c>
-      <c r="J606" s="1" t="s">
+      <c r="D606" s="3">
+        <v>1</v>
+      </c>
+      <c r="E606" s="3">
+        <v>2</v>
+      </c>
+      <c r="F606" s="3">
+        <v>1</v>
+      </c>
+      <c r="G606" s="3">
+        <v>1</v>
+      </c>
+      <c r="H606" s="3">
+        <v>0</v>
+      </c>
+      <c r="I606" s="3">
+        <v>0</v>
+      </c>
+      <c r="J606" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K606" s="1" t="s">
+      <c r="K606" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L606" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="607" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L606" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A607" t="s">
         <v>154</v>
       </c>
@@ -21154,73 +21157,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="608" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
+    <row r="608" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A608" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B608" t="s">
+      <c r="B608" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C608">
+      <c r="C608" s="1">
         <v>19</v>
       </c>
-      <c r="D608">
-        <v>1</v>
-      </c>
-      <c r="E608">
-        <v>2</v>
-      </c>
-      <c r="F608">
-        <v>1</v>
-      </c>
-      <c r="G608">
-        <v>3</v>
-      </c>
-      <c r="H608">
-        <v>0</v>
-      </c>
-      <c r="I608">
-        <v>0</v>
-      </c>
-      <c r="K608" t="s">
+      <c r="D608" s="1">
+        <v>1</v>
+      </c>
+      <c r="E608" s="1">
+        <v>2</v>
+      </c>
+      <c r="F608" s="1">
+        <v>1</v>
+      </c>
+      <c r="G608" s="1">
+        <v>3</v>
+      </c>
+      <c r="H608" s="1">
+        <v>0</v>
+      </c>
+      <c r="I608" s="1">
+        <v>0</v>
+      </c>
+      <c r="K608" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="L608">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="609" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
+      <c r="L608" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A609" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B609" t="s">
+      <c r="B609" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C609">
+      <c r="C609" s="1">
         <v>20</v>
       </c>
-      <c r="D609">
-        <v>1</v>
-      </c>
-      <c r="E609">
-        <v>2</v>
-      </c>
-      <c r="F609">
-        <v>1</v>
-      </c>
-      <c r="G609">
-        <v>4</v>
-      </c>
-      <c r="H609" t="s">
+      <c r="D609" s="1">
+        <v>1</v>
+      </c>
+      <c r="E609" s="1">
+        <v>2</v>
+      </c>
+      <c r="F609" s="1">
+        <v>1</v>
+      </c>
+      <c r="G609" s="1">
+        <v>4</v>
+      </c>
+      <c r="H609" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I609">
-        <v>0</v>
-      </c>
-      <c r="K609" t="s">
+      <c r="I609" s="1">
+        <v>0</v>
+      </c>
+      <c r="K609" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L609">
+      <c r="L609" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>